<commit_message>
modify henan 2/11 0-24
</commit_message>
<xml_diff>
--- a/NCP/data/unchecked/manual_collect/china/henan/henanCaseStatistics_20200211.xlsx
+++ b/NCP/data/unchecked/manual_collect/china/henan/henanCaseStatistics_20200211.xlsx
@@ -5,20 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\yiqing\data\henan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\yiqing\pkuvis.github.io\NCP\data\unchecked\manual_collect\china\henan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CFA801-E9CD-4ACE-9AE3-27019C0FD8A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17EAEE2-3B1B-4E7C-96A3-68360CDC26A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3288" yWindow="360" windowWidth="17280" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$AN$179</definedName>
+  </definedNames>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1142,10 +1151,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AN179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O166" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:AF179"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I182" sqref="I182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1402,7 +1412,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J3" s="2">
         <v>-1</v>
@@ -1464,7 +1474,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" hidden="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1536,7 +1546,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" hidden="1">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1608,7 +1618,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" hidden="1">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1680,7 +1690,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" hidden="1">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1752,7 +1762,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" hidden="1">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1824,7 +1834,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" hidden="1">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1896,7 +1906,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" hidden="1">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1968,7 +1978,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" hidden="1">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -2040,7 +2050,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" hidden="1">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -2112,7 +2122,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" hidden="1">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -2184,7 +2194,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" hidden="1">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -2256,7 +2266,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" hidden="1">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -2402,7 +2412,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:32" hidden="1">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -2474,7 +2484,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:32" hidden="1">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -2546,7 +2556,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:32" hidden="1">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -2618,7 +2628,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:32" hidden="1">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -2690,7 +2700,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:32" hidden="1">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -2762,7 +2772,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:32" hidden="1">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -2834,7 +2844,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:32" hidden="1">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2906,7 +2916,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:32">
+    <row r="24" spans="1:32" hidden="1">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2978,7 +2988,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:32" hidden="1">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -3124,7 +3134,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:32">
+    <row r="27" spans="1:32" hidden="1">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -3196,7 +3206,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:32">
+    <row r="28" spans="1:32" hidden="1">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -3268,7 +3278,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:32">
+    <row r="29" spans="1:32" hidden="1">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -3340,7 +3350,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:32">
+    <row r="30" spans="1:32" hidden="1">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -3412,7 +3422,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:32">
+    <row r="31" spans="1:32" hidden="1">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -3484,7 +3494,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:32">
+    <row r="32" spans="1:32" hidden="1">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -3556,7 +3566,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:32">
+    <row r="33" spans="1:32" hidden="1">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -3628,7 +3638,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:32">
+    <row r="34" spans="1:32" hidden="1">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -3700,7 +3710,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:32">
+    <row r="35" spans="1:32" hidden="1">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -3772,7 +3782,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:32">
+    <row r="36" spans="1:32" hidden="1">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -3844,7 +3854,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:32">
+    <row r="37" spans="1:32" hidden="1">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -3916,7 +3926,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:32">
+    <row r="38" spans="1:32" hidden="1">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -3988,7 +3998,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:32">
+    <row r="39" spans="1:32" hidden="1">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -4060,7 +4070,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:32">
+    <row r="40" spans="1:32" hidden="1">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -4132,7 +4142,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:32">
+    <row r="41" spans="1:32" hidden="1">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -4278,7 +4288,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:32">
+    <row r="43" spans="1:32" hidden="1">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -4350,7 +4360,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:32">
+    <row r="44" spans="1:32" hidden="1">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -4422,7 +4432,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:32">
+    <row r="45" spans="1:32" hidden="1">
       <c r="A45" s="2">
         <v>43</v>
       </c>
@@ -4494,7 +4504,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:32">
+    <row r="46" spans="1:32" hidden="1">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -4566,7 +4576,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:32">
+    <row r="47" spans="1:32" hidden="1">
       <c r="A47" s="2">
         <v>45</v>
       </c>
@@ -4638,7 +4648,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:32">
+    <row r="48" spans="1:32" hidden="1">
       <c r="A48" s="2">
         <v>46</v>
       </c>
@@ -4710,7 +4720,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:32">
+    <row r="49" spans="1:32" hidden="1">
       <c r="A49" s="2">
         <v>47</v>
       </c>
@@ -4782,7 +4792,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:32">
+    <row r="50" spans="1:32" hidden="1">
       <c r="A50" s="2">
         <v>48</v>
       </c>
@@ -4854,7 +4864,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:32">
+    <row r="51" spans="1:32" hidden="1">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -4926,7 +4936,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:32">
+    <row r="52" spans="1:32" hidden="1">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -5072,7 +5082,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:32">
+    <row r="54" spans="1:32" hidden="1">
       <c r="A54" s="2">
         <v>52</v>
       </c>
@@ -5144,7 +5154,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:32">
+    <row r="55" spans="1:32" hidden="1">
       <c r="A55" s="2">
         <v>53</v>
       </c>
@@ -5216,7 +5226,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:32">
+    <row r="56" spans="1:32" hidden="1">
       <c r="A56" s="2">
         <v>54</v>
       </c>
@@ -5288,7 +5298,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:32">
+    <row r="57" spans="1:32" hidden="1">
       <c r="A57" s="2">
         <v>55</v>
       </c>
@@ -5360,7 +5370,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:32">
+    <row r="58" spans="1:32" hidden="1">
       <c r="A58" s="2">
         <v>56</v>
       </c>
@@ -5432,7 +5442,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:32">
+    <row r="59" spans="1:32" hidden="1">
       <c r="A59" s="2">
         <v>57</v>
       </c>
@@ -5504,7 +5514,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:32">
+    <row r="60" spans="1:32" hidden="1">
       <c r="A60" s="2">
         <v>58</v>
       </c>
@@ -5576,7 +5586,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:32">
+    <row r="61" spans="1:32" hidden="1">
       <c r="A61" s="2">
         <v>59</v>
       </c>
@@ -5648,7 +5658,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:32">
+    <row r="62" spans="1:32" hidden="1">
       <c r="A62" s="2">
         <v>60</v>
       </c>
@@ -5794,7 +5804,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:32">
+    <row r="64" spans="1:32" hidden="1">
       <c r="A64" s="2">
         <v>62</v>
       </c>
@@ -5866,7 +5876,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:32">
+    <row r="65" spans="1:32" hidden="1">
       <c r="A65" s="2">
         <v>63</v>
       </c>
@@ -5938,7 +5948,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="1:32">
+    <row r="66" spans="1:32" hidden="1">
       <c r="A66" s="2">
         <v>64</v>
       </c>
@@ -6010,7 +6020,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:32">
+    <row r="67" spans="1:32" hidden="1">
       <c r="A67" s="2">
         <v>65</v>
       </c>
@@ -6082,7 +6092,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="1:32">
+    <row r="68" spans="1:32" hidden="1">
       <c r="A68" s="2">
         <v>66</v>
       </c>
@@ -6228,7 +6238,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="1:32">
+    <row r="70" spans="1:32" hidden="1">
       <c r="A70" s="2">
         <v>68</v>
       </c>
@@ -6300,7 +6310,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="71" spans="1:32">
+    <row r="71" spans="1:32" hidden="1">
       <c r="A71" s="2">
         <v>69</v>
       </c>
@@ -6372,7 +6382,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="1:32">
+    <row r="72" spans="1:32" hidden="1">
       <c r="A72" s="2">
         <v>70</v>
       </c>
@@ -6444,7 +6454,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:32">
+    <row r="73" spans="1:32" hidden="1">
       <c r="A73" s="2">
         <v>71</v>
       </c>
@@ -6516,7 +6526,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="74" spans="1:32">
+    <row r="74" spans="1:32" hidden="1">
       <c r="A74" s="2">
         <v>72</v>
       </c>
@@ -6588,7 +6598,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="1:32">
+    <row r="75" spans="1:32" hidden="1">
       <c r="A75" s="2">
         <v>73</v>
       </c>
@@ -6660,7 +6670,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="1:32">
+    <row r="76" spans="1:32" hidden="1">
       <c r="A76" s="2">
         <v>74</v>
       </c>
@@ -6732,7 +6742,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="1:32">
+    <row r="77" spans="1:32" hidden="1">
       <c r="A77" s="2">
         <v>75</v>
       </c>
@@ -6804,7 +6814,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:32">
+    <row r="78" spans="1:32" hidden="1">
       <c r="A78" s="2">
         <v>76</v>
       </c>
@@ -6876,7 +6886,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="1:32">
+    <row r="79" spans="1:32" hidden="1">
       <c r="A79" s="2">
         <v>77</v>
       </c>
@@ -6948,7 +6958,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="1:32">
+    <row r="80" spans="1:32" hidden="1">
       <c r="A80" s="2">
         <v>78</v>
       </c>
@@ -7020,7 +7030,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="1:32">
+    <row r="81" spans="1:32" hidden="1">
       <c r="A81" s="2">
         <v>79</v>
       </c>
@@ -7166,7 +7176,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="83" spans="1:32">
+    <row r="83" spans="1:32" hidden="1">
       <c r="A83" s="2">
         <v>81</v>
       </c>
@@ -7238,7 +7248,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="84" spans="1:32">
+    <row r="84" spans="1:32" hidden="1">
       <c r="A84" s="2">
         <v>82</v>
       </c>
@@ -7310,7 +7320,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="85" spans="1:32">
+    <row r="85" spans="1:32" hidden="1">
       <c r="A85" s="2">
         <v>83</v>
       </c>
@@ -7382,7 +7392,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="86" spans="1:32">
+    <row r="86" spans="1:32" hidden="1">
       <c r="A86" s="2">
         <v>84</v>
       </c>
@@ -7454,7 +7464,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="87" spans="1:32">
+    <row r="87" spans="1:32" hidden="1">
       <c r="A87" s="2">
         <v>85</v>
       </c>
@@ -7526,7 +7536,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="88" spans="1:32">
+    <row r="88" spans="1:32" hidden="1">
       <c r="A88" s="2">
         <v>86</v>
       </c>
@@ -7598,7 +7608,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="89" spans="1:32">
+    <row r="89" spans="1:32" hidden="1">
       <c r="A89" s="2">
         <v>87</v>
       </c>
@@ -7670,7 +7680,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="90" spans="1:32">
+    <row r="90" spans="1:32" hidden="1">
       <c r="A90" s="2">
         <v>88</v>
       </c>
@@ -7742,7 +7752,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="91" spans="1:32">
+    <row r="91" spans="1:32" hidden="1">
       <c r="A91" s="2">
         <v>89</v>
       </c>
@@ -7814,7 +7824,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="92" spans="1:32">
+    <row r="92" spans="1:32" hidden="1">
       <c r="A92" s="2">
         <v>90</v>
       </c>
@@ -7960,7 +7970,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="94" spans="1:32">
+    <row r="94" spans="1:32" hidden="1">
       <c r="A94" s="2">
         <v>92</v>
       </c>
@@ -8032,7 +8042,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="95" spans="1:32">
+    <row r="95" spans="1:32" hidden="1">
       <c r="A95" s="2">
         <v>93</v>
       </c>
@@ -8104,7 +8114,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="96" spans="1:32">
+    <row r="96" spans="1:32" hidden="1">
       <c r="A96" s="2">
         <v>94</v>
       </c>
@@ -8176,7 +8186,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="97" spans="1:32">
+    <row r="97" spans="1:32" hidden="1">
       <c r="A97" s="2">
         <v>95</v>
       </c>
@@ -8248,7 +8258,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="98" spans="1:32">
+    <row r="98" spans="1:32" hidden="1">
       <c r="A98" s="2">
         <v>96</v>
       </c>
@@ -8320,7 +8330,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="99" spans="1:32">
+    <row r="99" spans="1:32" hidden="1">
       <c r="A99" s="2">
         <v>97</v>
       </c>
@@ -8466,7 +8476,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="101" spans="1:32">
+    <row r="101" spans="1:32" hidden="1">
       <c r="A101" s="2">
         <v>99</v>
       </c>
@@ -8538,7 +8548,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="102" spans="1:32">
+    <row r="102" spans="1:32" hidden="1">
       <c r="A102" s="2">
         <v>100</v>
       </c>
@@ -8610,7 +8620,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:32">
+    <row r="103" spans="1:32" hidden="1">
       <c r="A103" s="2">
         <v>101</v>
       </c>
@@ -8682,7 +8692,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="104" spans="1:32">
+    <row r="104" spans="1:32" hidden="1">
       <c r="A104" s="2">
         <v>102</v>
       </c>
@@ -8754,7 +8764,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="105" spans="1:32">
+    <row r="105" spans="1:32" hidden="1">
       <c r="A105" s="2">
         <v>103</v>
       </c>
@@ -8826,7 +8836,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="106" spans="1:32">
+    <row r="106" spans="1:32" hidden="1">
       <c r="A106" s="2">
         <v>104</v>
       </c>
@@ -8972,7 +8982,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="108" spans="1:32">
+    <row r="108" spans="1:32" hidden="1">
       <c r="A108" s="2">
         <v>106</v>
       </c>
@@ -9044,7 +9054,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="109" spans="1:32">
+    <row r="109" spans="1:32" hidden="1">
       <c r="A109" s="2">
         <v>107</v>
       </c>
@@ -9116,7 +9126,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="110" spans="1:32">
+    <row r="110" spans="1:32" hidden="1">
       <c r="A110" s="2">
         <v>108</v>
       </c>
@@ -9188,7 +9198,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="111" spans="1:32">
+    <row r="111" spans="1:32" hidden="1">
       <c r="A111" s="2">
         <v>109</v>
       </c>
@@ -9260,7 +9270,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="112" spans="1:32">
+    <row r="112" spans="1:32" hidden="1">
       <c r="A112" s="2">
         <v>110</v>
       </c>
@@ -9406,7 +9416,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="114" spans="1:32">
+    <row r="114" spans="1:32" hidden="1">
       <c r="A114" s="2">
         <v>112</v>
       </c>
@@ -9478,7 +9488,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="115" spans="1:32">
+    <row r="115" spans="1:32" hidden="1">
       <c r="A115" s="2">
         <v>113</v>
       </c>
@@ -9550,7 +9560,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="116" spans="1:32">
+    <row r="116" spans="1:32" hidden="1">
       <c r="A116" s="2">
         <v>114</v>
       </c>
@@ -9622,7 +9632,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="117" spans="1:32">
+    <row r="117" spans="1:32" hidden="1">
       <c r="A117" s="2">
         <v>115</v>
       </c>
@@ -9694,7 +9704,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="118" spans="1:32">
+    <row r="118" spans="1:32" hidden="1">
       <c r="A118" s="2">
         <v>116</v>
       </c>
@@ -9766,7 +9776,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="119" spans="1:32">
+    <row r="119" spans="1:32" hidden="1">
       <c r="A119" s="2">
         <v>117</v>
       </c>
@@ -9910,7 +9920,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="121" spans="1:32">
+    <row r="121" spans="1:32" hidden="1">
       <c r="A121" s="2">
         <v>119</v>
       </c>
@@ -9982,7 +9992,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="122" spans="1:32">
+    <row r="122" spans="1:32" hidden="1">
       <c r="A122" s="2">
         <v>120</v>
       </c>
@@ -10054,7 +10064,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="123" spans="1:32">
+    <row r="123" spans="1:32" hidden="1">
       <c r="A123" s="2">
         <v>121</v>
       </c>
@@ -10126,7 +10136,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="124" spans="1:32">
+    <row r="124" spans="1:32" hidden="1">
       <c r="A124" s="2">
         <v>122</v>
       </c>
@@ -10198,7 +10208,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="125" spans="1:32">
+    <row r="125" spans="1:32" hidden="1">
       <c r="A125" s="2">
         <v>123</v>
       </c>
@@ -10270,7 +10280,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="126" spans="1:32">
+    <row r="126" spans="1:32" hidden="1">
       <c r="A126" s="2">
         <v>124</v>
       </c>
@@ -10342,7 +10352,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="127" spans="1:32">
+    <row r="127" spans="1:32" hidden="1">
       <c r="A127" s="2">
         <v>125</v>
       </c>
@@ -10414,7 +10424,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="128" spans="1:32">
+    <row r="128" spans="1:32" hidden="1">
       <c r="A128" s="2">
         <v>126</v>
       </c>
@@ -10486,7 +10496,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="129" spans="1:32">
+    <row r="129" spans="1:32" hidden="1">
       <c r="A129" s="2">
         <v>127</v>
       </c>
@@ -10558,7 +10568,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="130" spans="1:32">
+    <row r="130" spans="1:32" hidden="1">
       <c r="A130" s="2">
         <v>128</v>
       </c>
@@ -10630,7 +10640,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="131" spans="1:32">
+    <row r="131" spans="1:32" hidden="1">
       <c r="A131" s="2">
         <v>129</v>
       </c>
@@ -10702,7 +10712,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="132" spans="1:32">
+    <row r="132" spans="1:32" hidden="1">
       <c r="A132" s="2">
         <v>130</v>
       </c>
@@ -10774,7 +10784,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="133" spans="1:32">
+    <row r="133" spans="1:32" hidden="1">
       <c r="A133" s="2">
         <v>131</v>
       </c>
@@ -10920,7 +10930,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="135" spans="1:32">
+    <row r="135" spans="1:32" hidden="1">
       <c r="A135" s="2">
         <v>133</v>
       </c>
@@ -10992,7 +11002,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="136" spans="1:32">
+    <row r="136" spans="1:32" hidden="1">
       <c r="A136" s="2">
         <v>134</v>
       </c>
@@ -11064,7 +11074,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="137" spans="1:32">
+    <row r="137" spans="1:32" hidden="1">
       <c r="A137" s="2">
         <v>135</v>
       </c>
@@ -11136,7 +11146,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="138" spans="1:32">
+    <row r="138" spans="1:32" hidden="1">
       <c r="A138" s="2">
         <v>136</v>
       </c>
@@ -11208,7 +11218,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="139" spans="1:32">
+    <row r="139" spans="1:32" hidden="1">
       <c r="A139" s="2">
         <v>137</v>
       </c>
@@ -11280,7 +11290,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="140" spans="1:32">
+    <row r="140" spans="1:32" hidden="1">
       <c r="A140" s="2">
         <v>138</v>
       </c>
@@ -11352,7 +11362,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="141" spans="1:32">
+    <row r="141" spans="1:32" hidden="1">
       <c r="A141" s="2">
         <v>139</v>
       </c>
@@ -11424,7 +11434,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="142" spans="1:32">
+    <row r="142" spans="1:32" hidden="1">
       <c r="A142" s="2">
         <v>140</v>
       </c>
@@ -11496,7 +11506,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="143" spans="1:32">
+    <row r="143" spans="1:32" hidden="1">
       <c r="A143" s="2">
         <v>141</v>
       </c>
@@ -11642,7 +11652,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="145" spans="1:32">
+    <row r="145" spans="1:32" hidden="1">
       <c r="A145" s="2">
         <v>143</v>
       </c>
@@ -11714,7 +11724,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="146" spans="1:32">
+    <row r="146" spans="1:32" hidden="1">
       <c r="A146" s="2">
         <v>144</v>
       </c>
@@ -11786,7 +11796,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="147" spans="1:32">
+    <row r="147" spans="1:32" hidden="1">
       <c r="A147" s="2">
         <v>145</v>
       </c>
@@ -11858,7 +11868,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="148" spans="1:32">
+    <row r="148" spans="1:32" hidden="1">
       <c r="A148" s="2">
         <v>146</v>
       </c>
@@ -11930,7 +11940,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="149" spans="1:32">
+    <row r="149" spans="1:32" hidden="1">
       <c r="A149" s="2">
         <v>147</v>
       </c>
@@ -12002,7 +12012,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="150" spans="1:32">
+    <row r="150" spans="1:32" hidden="1">
       <c r="A150" s="2">
         <v>148</v>
       </c>
@@ -12074,7 +12084,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="151" spans="1:32">
+    <row r="151" spans="1:32" hidden="1">
       <c r="A151" s="2">
         <v>149</v>
       </c>
@@ -12146,7 +12156,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="152" spans="1:32">
+    <row r="152" spans="1:32" hidden="1">
       <c r="A152" s="2">
         <v>150</v>
       </c>
@@ -12218,7 +12228,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="153" spans="1:32">
+    <row r="153" spans="1:32" hidden="1">
       <c r="A153" s="2">
         <v>151</v>
       </c>
@@ -12290,7 +12300,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="154" spans="1:32">
+    <row r="154" spans="1:32" hidden="1">
       <c r="A154" s="2">
         <v>152</v>
       </c>
@@ -12436,7 +12446,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="156" spans="1:32">
+    <row r="156" spans="1:32" hidden="1">
       <c r="A156" s="2">
         <v>154</v>
       </c>
@@ -12508,7 +12518,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="157" spans="1:32">
+    <row r="157" spans="1:32" hidden="1">
       <c r="A157" s="2">
         <v>155</v>
       </c>
@@ -12580,7 +12590,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="158" spans="1:32">
+    <row r="158" spans="1:32" hidden="1">
       <c r="A158" s="2">
         <v>156</v>
       </c>
@@ -12652,7 +12662,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="159" spans="1:32">
+    <row r="159" spans="1:32" hidden="1">
       <c r="A159" s="2">
         <v>157</v>
       </c>
@@ -12724,7 +12734,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="160" spans="1:32">
+    <row r="160" spans="1:32" hidden="1">
       <c r="A160" s="2">
         <v>158</v>
       </c>
@@ -12796,7 +12806,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="161" spans="1:32">
+    <row r="161" spans="1:32" hidden="1">
       <c r="A161" s="2">
         <v>159</v>
       </c>
@@ -12868,7 +12878,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="162" spans="1:32">
+    <row r="162" spans="1:32" hidden="1">
       <c r="A162" s="2">
         <v>160</v>
       </c>
@@ -12940,7 +12950,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="163" spans="1:32">
+    <row r="163" spans="1:32" hidden="1">
       <c r="A163" s="2">
         <v>161</v>
       </c>
@@ -13012,7 +13022,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="164" spans="1:32">
+    <row r="164" spans="1:32" hidden="1">
       <c r="A164" s="2">
         <v>162</v>
       </c>
@@ -13084,7 +13094,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="165" spans="1:32">
+    <row r="165" spans="1:32" hidden="1">
       <c r="A165" s="2">
         <v>163</v>
       </c>
@@ -13230,7 +13240,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="167" spans="1:32">
+    <row r="167" spans="1:32" hidden="1">
       <c r="A167" s="2">
         <v>165</v>
       </c>
@@ -13302,7 +13312,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="168" spans="1:32">
+    <row r="168" spans="1:32" hidden="1">
       <c r="A168" s="2">
         <v>166</v>
       </c>
@@ -13374,7 +13384,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="169" spans="1:32">
+    <row r="169" spans="1:32" hidden="1">
       <c r="A169" s="2">
         <v>167</v>
       </c>
@@ -13446,7 +13456,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="170" spans="1:32">
+    <row r="170" spans="1:32" hidden="1">
       <c r="A170" s="2">
         <v>168</v>
       </c>
@@ -13518,7 +13528,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="171" spans="1:32">
+    <row r="171" spans="1:32" hidden="1">
       <c r="A171" s="2">
         <v>169</v>
       </c>
@@ -13590,7 +13600,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="172" spans="1:32">
+    <row r="172" spans="1:32" hidden="1">
       <c r="A172" s="2">
         <v>170</v>
       </c>
@@ -13662,7 +13672,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="173" spans="1:32">
+    <row r="173" spans="1:32" hidden="1">
       <c r="A173" s="2">
         <v>171</v>
       </c>
@@ -13734,7 +13744,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="174" spans="1:32">
+    <row r="174" spans="1:32" hidden="1">
       <c r="A174" s="2">
         <v>172</v>
       </c>
@@ -13806,7 +13816,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="175" spans="1:32">
+    <row r="175" spans="1:32" hidden="1">
       <c r="A175" s="2">
         <v>173</v>
       </c>
@@ -13878,7 +13888,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="176" spans="1:32">
+    <row r="176" spans="1:32" hidden="1">
       <c r="A176" s="2">
         <v>174</v>
       </c>
@@ -14181,6 +14191,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:AN179" xr:uid="{DC60BAC1-A73D-462F-A26A-6A95BD5A28B4}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="城市级"/>
+        <filter val="省级"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="V3" r:id="rId1" xr:uid="{140787E4-ED5F-423B-88A0-97D2AA8978CB}"/>
@@ -14362,5 +14380,6 @@
     <hyperlink ref="V178" r:id="rId177" xr:uid="{C1BDDEEC-CF02-4D2D-88E3-9414F42F71EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId178"/>
 </worksheet>
 </file>
</xml_diff>